<commit_message>
Changed baseurl parameter in the config
</commit_message>
<xml_diff>
--- a/member/members_v3.xlsx
+++ b/member/members_v3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
   <si>
     <t>Paul</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>Veerle de Herdt</t>
+  </si>
+  <si>
+    <t>Lisanne Canjels</t>
+  </si>
+  <si>
+    <t>Chris Baeken</t>
   </si>
 </sst>
 </file>
@@ -162,12 +168,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -182,8 +194,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,14 +477,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -583,6 +599,9 @@
       <c r="D9" t="s">
         <v>20</v>
       </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -605,6 +624,9 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -624,6 +646,9 @@
       <c r="B13">
         <v>12</v>
       </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -635,6 +660,9 @@
       <c r="D14" t="s">
         <v>20</v>
       </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -671,6 +699,9 @@
       <c r="D17" t="s">
         <v>20</v>
       </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -718,6 +749,9 @@
       <c r="D21" t="s">
         <v>20</v>
       </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -737,10 +771,13 @@
       <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>22</v>
       </c>
       <c r="D23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" t="s">
         <v>20</v>
       </c>
     </row>
@@ -748,84 +785,96 @@
       <c r="A24" t="s">
         <v>38</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25">
+        <v>41</v>
+      </c>
+      <c r="B25" s="1">
         <v>24</v>
       </c>
-      <c r="C25" t="s">
-        <v>35</v>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26">
+        <v>42</v>
+      </c>
+      <c r="B26" s="1">
         <v>25</v>
       </c>
       <c r="C26" t="s">
         <v>35</v>
       </c>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1">
         <v>26</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
       </c>
-      <c r="D27" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1">
         <v>27</v>
       </c>
       <c r="C28" t="s">
         <v>35</v>
       </c>
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1">
         <v>28</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
       </c>
+      <c r="D29" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30">
+        <v>31</v>
+      </c>
+      <c r="B30" s="1">
         <v>29</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
       </c>
+      <c r="E30" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31">
+        <v>37</v>
+      </c>
+      <c r="B31" s="1">
         <v>30</v>
       </c>
       <c r="C31" t="s">
@@ -834,26 +883,51 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32">
+        <v>39</v>
+      </c>
+      <c r="B32" s="1">
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="1">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="1">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>23</v>
       </c>
-      <c r="B33">
-        <v>32</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="B35" s="1">
+        <v>34</v>
+      </c>
+      <c r="D35" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Stephan to member
</commit_message>
<xml_diff>
--- a/member/members_v3.xlsx
+++ b/member/members_v3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
   <si>
     <t>Paul</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Chris Baeken</t>
+  </si>
+  <si>
+    <t>Stephan Heunis</t>
   </si>
 </sst>
 </file>
@@ -477,11 +480,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,21 +808,15 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1">
         <v>25</v>
       </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B27" s="1">
         <v>26</v>
@@ -827,10 +824,13 @@
       <c r="C27" t="s">
         <v>35</v>
       </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1">
         <v>27</v>
@@ -838,13 +838,10 @@
       <c r="C28" t="s">
         <v>35</v>
       </c>
-      <c r="E28" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1">
         <v>28</v>
@@ -852,13 +849,13 @@
       <c r="C29" t="s">
         <v>35</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B30" s="1">
         <v>29</v>
@@ -866,13 +863,13 @@
       <c r="C30" t="s">
         <v>35</v>
       </c>
-      <c r="E30" t="s">
+      <c r="D30" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1">
         <v>30</v>
@@ -880,10 +877,13 @@
       <c r="C31" t="s">
         <v>35</v>
       </c>
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1">
         <v>31</v>
@@ -891,13 +891,10 @@
       <c r="C32" t="s">
         <v>35</v>
       </c>
-      <c r="E32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="1">
         <v>32</v>
@@ -905,29 +902,43 @@
       <c r="C33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B34" s="1">
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B35" s="1">
         <v>34</v>
       </c>
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
       <c r="D35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="1">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>